<commit_message>
adding colors to parallel groups
</commit_message>
<xml_diff>
--- a/shipClassTests/testResults/sensedComp_MultiSensors.xlsx
+++ b/shipClassTests/testResults/sensedComp_MultiSensors.xlsx
@@ -7,48 +7,68 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sensed highRelSensors" sheetId="1" r:id="rId1"/>
+    <sheet name="Sensed Highrelsensors" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Time Step</t>
   </si>
   <si>
-    <t>Truth State</t>
-  </si>
-  <si>
-    <t>Sensor 1</t>
-  </si>
-  <si>
-    <t>Sensor 2</t>
-  </si>
-  <si>
-    <t>Sensor 3</t>
-  </si>
-  <si>
-    <t>Sensor 4</t>
+    <t>Comp Truth State</t>
+  </si>
+  <si>
+    <t>Sensor 1 Truth State</t>
+  </si>
+  <si>
+    <t>Sensor 2 Truth State</t>
+  </si>
+  <si>
+    <t>Sensor 3 Truth State</t>
+  </si>
+  <si>
+    <t>Sensor 4 Truth State</t>
   </si>
   <si>
     <t>Sensed State</t>
   </si>
   <si>
+    <t>Sensor 1 Reading from Comp</t>
+  </si>
+  <si>
+    <t>Sensor 2 Reading from Comp</t>
+  </si>
+  <si>
+    <t>Sensor 3 Reading from Comp</t>
+  </si>
+  <si>
+    <t>Sensor 4 Reading from Comp</t>
+  </si>
+  <si>
+    <t>Does Sensed State Match Truth State?</t>
+  </si>
+  <si>
     <t>Are Sensors Working?</t>
-  </si>
-  <si>
-    <t>Did Sensed State Match Truth State?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -64,10 +84,49 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -76,11 +135,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,46 +441,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="9" width="12.28515625" customWidth="1"/>
+    <col min="1" max="13" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2">
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="3">
         <v>0</v>
       </c>
       <c r="B2">
@@ -429,23 +510,35 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="4">
         <v>1</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="4">
+        <v>1</v>
+      </c>
+      <c r="L2" s="3">
+        <f>IF(B2 = G2, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
         <f>MODE(C2:F2)</f>
         <v>0</v>
       </c>
-      <c r="I2">
-        <f>IF(B2=G2, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3">
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
       <c r="B3">
@@ -460,23 +553,35 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3">
-        <v>1</v>
+      <c r="F3" s="4">
+        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3">
+        <f>IF(B3 = G3, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="3">
         <f>MODE(C3:F3)</f>
         <v>0</v>
       </c>
-      <c r="I3">
-        <f>IF(B3=G3, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4">
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
       <c r="B4">
@@ -491,23 +596,35 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>1</v>
+      <c r="F4" s="4">
+        <v>0</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3">
+        <f>IF(B4 = G4, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="3">
         <f>MODE(C4:F4)</f>
         <v>0</v>
       </c>
-      <c r="I4">
-        <f>IF(B4=G4, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5">
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
       <c r="B5">
@@ -520,25 +637,37 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
       <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3">
+        <f>IF(B5 = G5, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M5" s="3">
         <f>MODE(C5:F5)</f>
         <v>0</v>
       </c>
-      <c r="I5">
-        <f>IF(B5=G5, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6">
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
       <c r="B6">
@@ -551,25 +680,37 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
       <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
+        <v>1</v>
+      </c>
+      <c r="L6" s="3">
+        <f>IF(B6 = G6, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="3">
         <f>MODE(C6:F6)</f>
         <v>0</v>
       </c>
-      <c r="I6">
-        <f>IF(B6=G6, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7">
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
       <c r="B7">
@@ -582,118 +723,166 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
+        <v>1</v>
+      </c>
+      <c r="L7" s="3">
+        <f>IF(B7 = G7, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="3">
         <f>MODE(C7:F7)</f>
         <v>0</v>
       </c>
-      <c r="I7">
-        <f>IF(B7=G7, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8">
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
+        <v>1</v>
+      </c>
+      <c r="L8" s="3">
+        <f>IF(B8 = G8, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M8" s="3">
         <f>MODE(C8:F8)</f>
         <v>0</v>
       </c>
-      <c r="I8">
-        <f>IF(B8=G8, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9">
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9" s="4">
+        <v>1</v>
+      </c>
+      <c r="L9" s="3">
+        <f>IF(B9 = G9, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="3">
         <f>MODE(C9:F9)</f>
         <v>0</v>
       </c>
-      <c r="I9">
-        <f>IF(B9=G9, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10">
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
       <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3">
+        <f>IF(B10 = G10, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="3">
         <f>MODE(C10:F10)</f>
         <v>0</v>
       </c>
-      <c r="I10">
-        <f>IF(B10=G10, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
-      <c r="A11">
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11">
@@ -706,25 +895,37 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>1</v>
+      </c>
+      <c r="L11" s="3">
+        <f>IF(B11 = G11, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="3">
         <f>MODE(C11:F11)</f>
         <v>0</v>
       </c>
-      <c r="I11">
-        <f>IF(B11=G11, 1, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12">
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12">
@@ -737,25 +938,37 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
       <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>1</v>
+      </c>
+      <c r="L12" s="3">
+        <f>IF(B12 = G12, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="M12" s="3">
         <f>MODE(C12:F12)</f>
         <v>0</v>
       </c>
-      <c r="I12">
-        <f>IF(B12=G12, 1, 0)</f>
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H2:H12">
+  <conditionalFormatting sqref="L2:L12">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min" val="0"/>
@@ -765,12 +978,14 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I12">
+  <conditionalFormatting sqref="M2:M12">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
         <cfvo type="max" val="0"/>
         <color rgb="FFFD0000"/>
+        <color rgb="FFFFFF00"/>
         <color rgb="FF00FD00"/>
       </colorScale>
     </cfRule>

</xml_diff>